<commit_message>
VerifyFooter -  MainPageTest_VerifyFooter - COMPLETE
</commit_message>
<xml_diff>
--- a/Test Cases - Excel Files/Scenariusz Testowy - Weryfikacja zakładki kontakt.xlsx
+++ b/Test Cases - Excel Files/Scenariusz Testowy - Weryfikacja zakładki kontakt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\Documents\GitHub\Selenium-Project-Online-Store-Tests\Test Cases - Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B32D432-C1C5-41D4-BFAC-C9559B6F4F5F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA470A7-5795-420B-ADB6-593929BEC599}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -130,24 +130,27 @@
     <t>Autor Scenariusza Testowego</t>
   </si>
   <si>
-    <t>Wejdź na główną stronę sklepu i zweryfikuj tytuł strony</t>
-  </si>
-  <si>
     <t>Adres głównej strony sklepu: http://koszulkifootball.sellingo.pl/
 Poprawny tytuł strony to: 'Koszulkifootball.sellingo.pl'</t>
   </si>
   <si>
+    <t>Poprawny tytuł strony to: 'Kontakt'</t>
+  </si>
+  <si>
+    <t>Wejdź na główną stronę sklepu, usuń pliki cookies i zweryfikuj tytuł strony. Dodatkowo wykonaj zrzut ekranu.</t>
+  </si>
+  <si>
     <t>Strona główna sklepu wyświetlona
-Tytuł strony: ''Koszulkifootball.sellingo.pl''</t>
-  </si>
-  <si>
-    <t>Kliknij w zakładkę "Kontakt' i zweryfikuj tytuł strony</t>
-  </si>
-  <si>
-    <t>Poprawny tytuł strony to: 'Kontakt'</t>
-  </si>
-  <si>
-    <t>Użytkownik zostaje przeniesiony na podstronę 'Kontakt'. Tytuł strony: 'Kontakt'</t>
+Tytuł strony: ''Koszulkifootball.sellingo.pl''
+Pliki Cookies usunięte
+Zrzut ekranu zapisany do pliku .jpg</t>
+  </si>
+  <si>
+    <t>Kliknij w zakładkę "Kontakt' i zweryfikuj tytuł  strony.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Użytkownik zostaje przeniesiony na podstronę 'Kontakt'. Tytuł strony: 'Kontakt'
+</t>
   </si>
 </sst>
 </file>
@@ -549,6 +552,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -567,15 +579,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -893,7 +896,7 @@
   <dimension ref="B2:H998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -910,56 +913,56 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="11" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="13"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="16"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16" t="s">
+      <c r="C3" s="18"/>
+      <c r="D3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="18"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="21"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="16" t="s">
+      <c r="C4" s="18"/>
+      <c r="D4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="18"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="21"/>
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="16" t="s">
+      <c r="C5" s="18"/>
+      <c r="D5" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="18"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="21"/>
     </row>
     <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
@@ -985,22 +988,22 @@
       </c>
     </row>
     <row r="7" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="23" t="s">
+      <c r="E7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="13" t="s">
         <v>14</v>
       </c>
       <c r="H7" s="6" t="s">
@@ -1008,7 +1011,7 @@
       </c>
     </row>
     <row r="8" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1029,14 +1032,14 @@
       </c>
     </row>
     <row r="9" spans="2:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>41</v>
@@ -1052,7 +1055,7 @@
       </c>
     </row>
     <row r="10" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="11" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1075,7 +1078,7 @@
       </c>
     </row>
     <row r="11" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1098,7 +1101,7 @@
       </c>
     </row>
     <row r="12" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1121,7 +1124,7 @@
       </c>
     </row>
     <row r="13" spans="2:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="11" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="8" t="s">

</xml_diff>